<commit_message>
perubahan upload data karyawan
</commit_message>
<xml_diff>
--- a/assets/upload/upload_pegawai.xlsx
+++ b/assets/upload/upload_pegawai.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="125">
   <si>
     <t>No.</t>
   </si>
@@ -93,15 +93,6 @@
     <t>Nomor PKWT</t>
   </si>
   <si>
-    <t>Promosi Jabatan</t>
-  </si>
-  <si>
-    <t>Mutasi Jabatan</t>
-  </si>
-  <si>
-    <t>Demosi Jabatan</t>
-  </si>
-  <si>
     <t>Employment Status</t>
   </si>
   <si>
@@ -111,18 +102,12 @@
     <t>Join Date</t>
   </si>
   <si>
-    <t>Length of service</t>
-  </si>
-  <si>
     <t>Kelompok Jabatan</t>
   </si>
   <si>
     <t>Gol KJ</t>
   </si>
   <si>
-    <t>Latest Promotion</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -144,9 +129,6 @@
     <t>Single</t>
   </si>
   <si>
-    <t>BLOK KAMIS, RT 004/RW 002, KEL. MAJA UTARA, KEC. MAJA</t>
-  </si>
-  <si>
     <t>0821-1285-0847</t>
   </si>
   <si>
@@ -180,18 +162,9 @@
     <t>TK/0</t>
   </si>
   <si>
-    <t>LAJANG</t>
-  </si>
-  <si>
-    <t>Permanent Employee</t>
-  </si>
-  <si>
     <t>SPA</t>
   </si>
   <si>
-    <t>4years9months</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -201,33 +174,233 @@
     <t>3E-4D</t>
   </si>
   <si>
-    <t>01 Januari 2017</t>
-  </si>
-  <si>
-    <t>Dasep</t>
-  </si>
-  <si>
     <t>Employee No / NPK</t>
   </si>
   <si>
     <t>Education Join</t>
   </si>
   <si>
-    <t>Education Update</t>
-  </si>
-  <si>
-    <t>SMA</t>
+    <t>Murry</t>
+  </si>
+  <si>
+    <t>Febriansyah</t>
+  </si>
+  <si>
+    <t>Putra</t>
+  </si>
+  <si>
+    <t>Muray</t>
+  </si>
+  <si>
+    <t>Mursky</t>
+  </si>
+  <si>
+    <t>Koperasi</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>Operational</t>
+  </si>
+  <si>
+    <t>GA &amp; IT</t>
+  </si>
+  <si>
+    <t>HC Ops</t>
+  </si>
+  <si>
+    <t>Operational 1&amp;2</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>Koperasi Staff</t>
+  </si>
+  <si>
+    <t>HC Ops Staff</t>
+  </si>
+  <si>
+    <t>Operational 1&amp;2 Staff</t>
+  </si>
+  <si>
+    <t>GA Dept Head</t>
+  </si>
+  <si>
+    <t>Bogor</t>
+  </si>
+  <si>
+    <t>Jakarta 1</t>
+  </si>
+  <si>
+    <t>JL. WARAKAS IV GG.14 NO.30 RT.011 RW.011</t>
+  </si>
+  <si>
+    <t>0857-1961-1157</t>
+  </si>
+  <si>
+    <t>0812-9511-9022</t>
+  </si>
+  <si>
+    <t>0857-1625-3963</t>
+  </si>
+  <si>
+    <t>0857-1049-8174</t>
+  </si>
+  <si>
+    <t>b@gmail.com</t>
+  </si>
+  <si>
+    <t>c@gmail.com</t>
+  </si>
+  <si>
+    <t>d@gmail.com</t>
+  </si>
+  <si>
+    <t>e@gmail.com</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>3175042312881014</t>
+  </si>
+  <si>
+    <t>3175042312881016</t>
+  </si>
+  <si>
+    <t>3175042312881017</t>
+  </si>
+  <si>
+    <t>3175042312881018</t>
+  </si>
+  <si>
+    <t>3175042312881089</t>
+  </si>
+  <si>
+    <t>3175042312881090</t>
+  </si>
+  <si>
+    <t>3175042312881091</t>
+  </si>
+  <si>
+    <t>3175042312881094</t>
+  </si>
+  <si>
+    <t>000123678801</t>
+  </si>
+  <si>
+    <t>000122789711</t>
+  </si>
+  <si>
+    <t>000121900621</t>
+  </si>
+  <si>
+    <t>000121011531</t>
+  </si>
+  <si>
+    <t>120J12346</t>
+  </si>
+  <si>
+    <t>120J12347</t>
+  </si>
+  <si>
+    <t>120J12348</t>
+  </si>
+  <si>
+    <t>120J12349</t>
+  </si>
+  <si>
+    <t>0001G31219801</t>
+  </si>
+  <si>
+    <t>0001G31219802</t>
+  </si>
+  <si>
+    <t>0001G31219803</t>
+  </si>
+  <si>
+    <t>0001G31219804</t>
+  </si>
+  <si>
+    <t>961855236024000</t>
+  </si>
+  <si>
+    <t>546470865071000</t>
+  </si>
+  <si>
+    <t>679093351438000</t>
+  </si>
+  <si>
+    <t>Bank Permata</t>
+  </si>
+  <si>
+    <t>Bank Mandiri</t>
+  </si>
+  <si>
+    <t>1227536620</t>
+  </si>
+  <si>
+    <t>9000012611290</t>
+  </si>
+  <si>
+    <t>1220466821</t>
+  </si>
+  <si>
+    <t>4180279488</t>
+  </si>
+  <si>
+    <t>K/1</t>
+  </si>
+  <si>
+    <t>K/0</t>
+  </si>
+  <si>
+    <t>K/2</t>
+  </si>
+  <si>
+    <t>K/3</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Kontrak Employee</t>
+  </si>
+  <si>
+    <t>sgp</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Admin 2</t>
+  </si>
+  <si>
+    <t>Department Head</t>
+  </si>
+  <si>
+    <t>2F-3F</t>
+  </si>
+  <si>
+    <t>4D-5B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,13 +424,6 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -310,12 +476,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -338,12 +504,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
@@ -358,38 +539,50 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -401,6 +594,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -479,6 +677,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -513,6 +712,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -688,18 +888,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AF6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -722,29 +922,23 @@
     <col min="24" max="24" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.42578125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="1"/>
+    <col min="27" max="27" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.42578125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="25.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -783,40 +977,40 @@
       <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="AB1" s="3" t="s">
@@ -825,142 +1019,504 @@
       <c r="AC1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:32" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>220927</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="14">
+        <v>35840</v>
+      </c>
+      <c r="L2" s="15">
+        <v>22</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="6" t="s">
+      <c r="P2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="11">
+        <v>123456</v>
+      </c>
+      <c r="AA2" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" s="17">
+        <v>42461</v>
+      </c>
+      <c r="AD2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF2" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19">
+        <v>220928</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="14">
+        <v>35840</v>
+      </c>
+      <c r="L3" s="15">
+        <v>22</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z3" s="11">
+        <v>123456</v>
+      </c>
+      <c r="AA3" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" s="17">
+        <v>43525</v>
+      </c>
+      <c r="AD3" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE3" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF3" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>220929</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="14">
+        <v>35840</v>
+      </c>
+      <c r="L4" s="15">
+        <v>22</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="X4" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z4" s="11">
+        <v>123456</v>
+      </c>
+      <c r="AA4" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC4" s="17">
+        <v>43313</v>
+      </c>
+      <c r="AD4" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE4" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF4" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19">
+        <v>220930</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="F5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="14">
+        <v>35840</v>
+      </c>
+      <c r="L5" s="15">
+        <v>22</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="U5" s="11">
+        <v>0</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y5" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z5" s="11">
+        <v>123456</v>
+      </c>
+      <c r="AA5" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB5" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC5" s="17">
+        <v>40026</v>
+      </c>
+      <c r="AD5" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE5" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF5" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>220931</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="AJ1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" s="2" customFormat="1">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
+      <c r="F6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="14">
+        <v>35840</v>
+      </c>
+      <c r="L6" s="15">
+        <v>22</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="V6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="X6" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y6" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z6" s="11">
         <v>123456</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="17">
-        <v>35339</v>
-      </c>
-      <c r="L2" s="13">
-        <v>51</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z2" s="12">
-        <v>123456</v>
-      </c>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF2" s="18">
-        <v>42461</v>
-      </c>
-      <c r="AG2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH2" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI2" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ2" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL2" s="10" t="s">
-        <v>61</v>
+      <c r="AA6" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB6" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC6" s="17">
+        <v>41030</v>
+      </c>
+      <c r="AD6" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE6" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF6" s="16" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -969,24 +1525,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
perapihan form upload karyawan
</commit_message>
<xml_diff>
--- a/assets/upload/upload_pegawai.xlsx
+++ b/assets/upload/upload_pegawai.xlsx
@@ -398,7 +398,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -566,7 +566,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -575,7 +575,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -892,7 +892,7 @@
   <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AF6"/>
+      <selection activeCell="A7" sqref="A7:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
hhitung total umur karywan
</commit_message>
<xml_diff>
--- a/assets/upload/upload_pegawai.xlsx
+++ b/assets/upload/upload_pegawai.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="94">
   <si>
     <t>No.</t>
   </si>
@@ -111,18 +111,6 @@
     <t>a@gmail.com</t>
   </si>
   <si>
-    <t>3175042312881012</t>
-  </si>
-  <si>
-    <t>3175042312881088</t>
-  </si>
-  <si>
-    <t>000124567891</t>
-  </si>
-  <si>
-    <t>120J12345</t>
-  </si>
-  <si>
     <t>0001G31219800</t>
   </si>
   <si>
@@ -192,9 +180,6 @@
     <t>SMK DWIPA</t>
   </si>
   <si>
-    <t>Murry</t>
-  </si>
-  <si>
     <t>Head Offie</t>
   </si>
   <si>
@@ -213,18 +198,6 @@
     <t>AB</t>
   </si>
   <si>
-    <t>3175042312881111</t>
-  </si>
-  <si>
-    <t>3175042312881089</t>
-  </si>
-  <si>
-    <t>000124567892</t>
-  </si>
-  <si>
-    <t>120J12344</t>
-  </si>
-  <si>
     <t>0001G31219801</t>
   </si>
   <si>
@@ -237,9 +210,6 @@
     <t>KAWIN</t>
   </si>
   <si>
-    <t>SMK</t>
-  </si>
-  <si>
     <t>Operational</t>
   </si>
   <si>
@@ -255,17 +225,89 @@
     <t xml:space="preserve">SMAN 1 </t>
   </si>
   <si>
-    <t>Febriansyah</t>
+    <t>Risma</t>
+  </si>
+  <si>
+    <t>Rama Hidayat</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Ranti</t>
+  </si>
+  <si>
+    <t>Bayu Adji</t>
+  </si>
+  <si>
+    <t>3175042312881081</t>
+  </si>
+  <si>
+    <t>3175042312881080</t>
+  </si>
+  <si>
+    <t>3175042312881083</t>
+  </si>
+  <si>
+    <t>3175042312881084</t>
+  </si>
+  <si>
+    <t>3175042312881113</t>
+  </si>
+  <si>
+    <t>3175042312881010</t>
+  </si>
+  <si>
+    <t>3175042312881114</t>
+  </si>
+  <si>
+    <t>3175042312881115</t>
+  </si>
+  <si>
+    <t>000124567894</t>
+  </si>
+  <si>
+    <t>000124567895</t>
+  </si>
+  <si>
+    <t>000124567899</t>
+  </si>
+  <si>
+    <t>000124567856</t>
+  </si>
+  <si>
+    <t>12012345</t>
+  </si>
+  <si>
+    <t>12012346</t>
+  </si>
+  <si>
+    <t>12012340</t>
+  </si>
+  <si>
+    <t>12012341</t>
+  </si>
+  <si>
+    <t>6930347993</t>
+  </si>
+  <si>
+    <t>6930347992</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>S2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,7 +401,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,6 +457,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,11 +470,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -508,7 +548,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -543,7 +582,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -719,14 +757,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
@@ -736,7 +774,7 @@
     <col min="6" max="6" width="15.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="57.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="5" customWidth="1"/>
     <col min="10" max="10" width="5" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -763,12 +801,12 @@
     <col min="34" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -786,7 +824,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -840,39 +878,39 @@
         <v>22</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" s="21" t="s">
-        <v>52</v>
-      </c>
       <c r="AE1" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="14" customFormat="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="7">
-        <v>220212</v>
+        <v>220556</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>25</v>
@@ -887,10 +925,10 @@
         <v>28</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I2" s="8">
-        <v>36251</v>
+        <v>29312</v>
       </c>
       <c r="J2" s="9">
         <v>51</v>
@@ -904,79 +942,79 @@
       <c r="M2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="R2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="T2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="U2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="V2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="W2" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="X2" s="12">
         <v>123456</v>
       </c>
       <c r="Y2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="AA2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>49</v>
-      </c>
       <c r="AC2" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AD2" s="17">
         <v>41955</v>
       </c>
       <c r="AE2" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AF2" s="6">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="AG2" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="A3" s="22">
         <v>2</v>
       </c>
       <c r="B3" s="22">
-        <v>220220</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>58</v>
+        <v>565655</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>26</v>
@@ -985,85 +1023,287 @@
         <v>27</v>
       </c>
       <c r="G3" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="8">
+        <v>32611</v>
+      </c>
+      <c r="J3" s="22">
+        <v>6</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="P3" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q3" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="R3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="S3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="8">
-        <v>35898</v>
-      </c>
-      <c r="J3" s="22">
-        <v>21</v>
-      </c>
-      <c r="K3" s="24" t="s">
+      <c r="T3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="V3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="M3" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="T3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="U3" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="V3" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="X3" s="12">
         <v>123457</v>
       </c>
       <c r="Y3" s="13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Z3" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA3" s="23" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="AB3" s="19" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="AC3" s="20" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="AD3" s="17">
         <v>40853</v>
       </c>
       <c r="AE3" s="23" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="AF3" s="22">
         <v>2015</v>
       </c>
       <c r="AG3" s="23" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22">
+        <v>225655</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="8">
+        <v>32611</v>
+      </c>
+      <c r="J4" s="22">
+        <v>6</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="O4" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="P4" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q4" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="X4" s="12">
+        <v>123457</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z4" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA4" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB4" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD4" s="17">
+        <v>40853</v>
+      </c>
+      <c r="AE4" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF4" s="22">
+        <v>2015</v>
+      </c>
+      <c r="AG4" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22">
+        <v>552552</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="8">
+        <v>34802</v>
+      </c>
+      <c r="J5" s="22">
+        <v>6</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="X5" s="12">
+        <v>123457</v>
+      </c>
+      <c r="Y5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z5" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA5" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB5" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC5" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD5" s="17">
+        <v>40853</v>
+      </c>
+      <c r="AE5" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF5" s="22">
+        <v>2015</v>
+      </c>
+      <c r="AG5" s="23" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1073,26 +1313,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
perubahan vendor phpexcel to phpspreadsheet
</commit_message>
<xml_diff>
--- a/assets/upload/upload_pegawai.xlsx
+++ b/assets/upload/upload_pegawai.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murry Febriansyah P\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\master_ho\assets\upload\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
   <si>
     <t>No.</t>
   </si>
@@ -95,6 +95,9 @@
     <t>Kelompok Jabatan</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>Head Office</t>
   </si>
   <si>
@@ -107,9 +110,36 @@
     <t>BLOK KAMIS, RT 004/RW 002, KEL. MAJA UTARA, KEC. MAJA</t>
   </si>
   <si>
+    <t>0821-1285-0847</t>
+  </si>
+  <si>
+    <t>a@gmail.com</t>
+  </si>
+  <si>
+    <t>3175042312881012</t>
+  </si>
+  <si>
+    <t>3175042312881088</t>
+  </si>
+  <si>
+    <t>000124567891</t>
+  </si>
+  <si>
+    <t>120J12345</t>
+  </si>
+  <si>
+    <t>0001G31219800</t>
+  </si>
+  <si>
+    <t>246155097024000</t>
+  </si>
+  <si>
     <t>Bank Central Asia</t>
   </si>
   <si>
+    <t>6930347998</t>
+  </si>
+  <si>
     <t>TK/0</t>
   </si>
   <si>
@@ -119,12 +149,21 @@
     <t>Permanent Employee</t>
   </si>
   <si>
+    <t>Junior Analyst</t>
+  </si>
+  <si>
+    <t>Dasep</t>
+  </si>
+  <si>
     <t>Employee No / NPK</t>
   </si>
   <si>
     <t>Education Join</t>
   </si>
   <si>
+    <t>SMA</t>
+  </si>
+  <si>
     <t>Alamat KTP</t>
   </si>
   <si>
@@ -134,6 +173,15 @@
     <t>Kontak Darurat</t>
   </si>
   <si>
+    <t>Priuk Jakarta Utara</t>
+  </si>
+  <si>
+    <t>01212121212</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
     <t>Join Date</t>
   </si>
   <si>
@@ -146,15 +194,33 @@
     <t>Nama Sekolah / Kampus</t>
   </si>
   <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>SMK DWIPA</t>
+  </si>
+  <si>
     <t>Murry</t>
   </si>
   <si>
+    <t>Head Offie</t>
+  </si>
+  <si>
+    <t>Lodan Dalam II C RT 06 / RW 08 KEL.ANCOL JAKARTA UTARA</t>
+  </si>
+  <si>
     <t>Bandung</t>
   </si>
   <si>
     <t>0812-1212-2244</t>
   </si>
   <si>
+    <t>murrry@gmail.com</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
     <t>3175042312881111</t>
   </si>
   <si>
@@ -176,6 +242,9 @@
     <t>6930347991</t>
   </si>
   <si>
+    <t>KAWIN</t>
+  </si>
+  <si>
     <t>SMK</t>
   </si>
   <si>
@@ -198,21 +267,14 @@
   </si>
   <si>
     <t>sigap.png</t>
-  </si>
-  <si>
-    <t>b@gmail.com</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -308,7 +370,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -324,16 +386,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -350,10 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +751,7 @@
     <col min="7" max="7" width="57.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="5" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
@@ -710,7 +782,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -728,7 +800,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -782,135 +854,239 @@
         <v>22</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD1" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="9">
+        <v>36251</v>
+      </c>
+      <c r="J2" s="10">
+        <v>51</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="R2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="T2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="U2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="V2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="W2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="X2" s="13">
+        <v>123456</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" s="18">
+        <v>41955</v>
+      </c>
+      <c r="AE2" s="19" t="s">
         <v>57</v>
       </c>
+      <c r="AF2" s="6">
+        <v>2017</v>
+      </c>
+      <c r="AG2" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH2" s="19" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B3" s="23">
         <v>220220</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="9">
+        <v>35898</v>
+      </c>
+      <c r="J3" s="23">
+        <v>21</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="X3" s="13">
+        <v>123457</v>
+      </c>
+      <c r="Y3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="19">
-        <v>35898</v>
-      </c>
-      <c r="J2" s="7">
-        <v>23</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="X2" s="9">
-        <v>789101</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA2" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB2" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC2" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD2" s="11">
+      <c r="Z3" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA3" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC3" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD3" s="18">
         <v>40853</v>
       </c>
-      <c r="AE2" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" s="16">
+      <c r="AE3" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF3" s="23">
         <v>2015</v>
       </c>
-      <c r="AG2" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH2" s="12" t="s">
-        <v>58</v>
+      <c r="AG3" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH3" s="19" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>